<commit_message>
update ready for publish
</commit_message>
<xml_diff>
--- a/Emergency Department/ED model testing - Beta feedback.xlsx
+++ b/Emergency Department/ED model testing - Beta feedback.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\irnhsft.local\monitor\Redirected\Paul.Bullard\Documents\GitHub\EDDemandandCapacity\Emergency Department\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAD93BBE-6F13-400B-9171-FC9E04CD764A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F722850A-6594-4E01-9779-35905677C0E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DBDA8E0D-CBD9-4740-B6ED-34A08F0FE389}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{DBDA8E0D-CBD9-4740-B6ED-34A08F0FE389}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
   <si>
     <t>Feedback</t>
   </si>
@@ -222,15 +222,9 @@
     <t>Data Validation created for stream name to ensure no punctuation can be entered</t>
   </si>
   <si>
-    <t>Team to design templates for users to enter their own forecasting in to.</t>
-  </si>
-  <si>
     <t>Shift configuration does not account for statutory meal breaks</t>
   </si>
   <si>
-    <t>To be confirmed</t>
-  </si>
-  <si>
     <t>Shift Unfilled should also be an option on each daily entry</t>
   </si>
   <si>
@@ -273,10 +267,6 @@
     <t>Key added to Summary table</t>
   </si>
   <si>
-    <t>Legend added to chart.
-Wording to be completed.</t>
-  </si>
-  <si>
     <t>Step by step info added to forecasting app</t>
   </si>
   <si>
@@ -284,6 +274,18 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>Templates for users to enter their own forecasting in to created.</t>
+  </si>
+  <si>
+    <t>Legend added to chart.</t>
+  </si>
+  <si>
+    <t>Longer term forecasting required for job planning</t>
+  </si>
+  <si>
+    <t>Alternative forecasting methods to enable longer term planning being scoped.</t>
   </si>
 </sst>
 </file>
@@ -339,7 +341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -577,11 +579,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -596,9 +637,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -628,13 +666,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -648,19 +679,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -673,15 +694,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -708,6 +723,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -726,14 +750,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1050,428 +1079,438 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A938E1F3-58C3-4661-9FC6-857CF55C04F0}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B1:E44"/>
+  <dimension ref="B1:E45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="94.140625" customWidth="1"/>
-    <col min="4" max="4" width="117.140625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="103.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="94.1796875" customWidth="1"/>
+    <col min="4" max="4" width="117.1796875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="103.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="8.4499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" ht="8.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="21"/>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="22"/>
+      <c r="C4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25"/>
-      <c r="C3" t="s">
+    <row r="5" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="23"/>
+      <c r="C5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="27"/>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="28" t="s">
+    <row r="6" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="7" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="57" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B8" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
-      <c r="C9" s="11" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B9" s="51"/>
+      <c r="C9" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="59"/>
-      <c r="C10" s="8" t="s">
+    <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="52"/>
+      <c r="C10" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="44" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="2"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="57" t="s">
+    <row r="12" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B12" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E12" s="29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="58"/>
+    <row r="13" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="51"/>
       <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="58"/>
-      <c r="C14" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="43" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="58"/>
-      <c r="C15" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="59"/>
-      <c r="C16" s="45" t="s">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B14" s="51"/>
+      <c r="C14" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="45"/>
+      <c r="E14" s="46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15" s="51"/>
+      <c r="C15" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="45"/>
+      <c r="E15" s="46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="52"/>
+      <c r="C16" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="47" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="36"/>
+      <c r="E16" s="37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B17" s="2"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="57" t="s">
+    <row r="18" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="58"/>
-      <c r="C19" s="11" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B19" s="51"/>
+      <c r="C19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="58"/>
-      <c r="C20" s="48" t="s">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B20" s="51"/>
+      <c r="C20" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="38"/>
+      <c r="E20" s="39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B21" s="51"/>
+      <c r="C21" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49" t="s">
+      <c r="D21" s="38"/>
+      <c r="E21" s="39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B22" s="51"/>
+      <c r="C22" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="52"/>
+      <c r="C23" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="40"/>
+      <c r="E23" s="41" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="58"/>
-      <c r="C21" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="49" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" s="58"/>
-      <c r="C22" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" s="23"/>
-      <c r="E22" s="41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="59"/>
-      <c r="C23" s="50" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="50"/>
-      <c r="E23" s="51" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="2"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B25" s="57" t="s">
+    <row r="25" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" s="58"/>
-      <c r="C26" s="31" t="s">
+    <row r="26" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="51"/>
+      <c r="C26" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D26" s="31"/>
-      <c r="E26" s="40" t="s">
+      <c r="D26" s="27"/>
+      <c r="E26" s="32" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="59"/>
-      <c r="C27" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" s="15"/>
-      <c r="E27" s="6" t="s">
+    <row r="27" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="52"/>
+      <c r="C27" s="36" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="40"/>
+      <c r="E27" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="2"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B29" s="57" t="s">
+    <row r="29" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B29" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="37" t="s">
+      <c r="E29" s="29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B30" s="58"/>
-      <c r="C30" s="11" t="s">
+    <row r="30" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B30" s="51"/>
+      <c r="C30" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="11"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="59"/>
-      <c r="C31" s="21" t="s">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B31" s="56"/>
+      <c r="C31" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="57"/>
+      <c r="E31" s="58" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="52"/>
+      <c r="C32" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D31" s="38" t="s">
+      <c r="D32" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="39" t="s">
+      <c r="E32" s="31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="2:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="57" t="s">
+    <row r="33" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="2"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="2:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C34" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D34" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E34" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B34" s="58"/>
-      <c r="C34" s="17" t="s">
+    <row r="35" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B35" s="51"/>
+      <c r="C35" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="20" t="s">
+      <c r="D35" s="12"/>
+      <c r="E35" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="59"/>
-      <c r="C35" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="46"/>
-      <c r="E35" s="53" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="1"/>
-      <c r="E36" s="3"/>
-    </row>
-    <row r="37" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="33" t="s">
+    <row r="36" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="52"/>
+      <c r="C36" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="36"/>
+      <c r="E36" s="43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D37" s="1"/>
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="34" t="s">
+      <c r="C38" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D38" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="E37" s="36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="54" t="s">
+      <c r="E38" s="55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B40" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="9" t="s">
+      <c r="C40" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="10" t="s">
+      <c r="D40" s="8"/>
+      <c r="E40" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B40" s="55"/>
-      <c r="C40" s="11" t="s">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B41" s="48"/>
+      <c r="C41" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="12" t="s">
+      <c r="D41" s="10"/>
+      <c r="E41" s="11" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="55"/>
-      <c r="C41" s="11" t="s">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B42" s="48"/>
+      <c r="C42" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12" t="s">
+      <c r="D42" s="10"/>
+      <c r="E42" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="55"/>
-      <c r="C42" s="14" t="s">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="48"/>
+      <c r="C43" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="12" t="s">
+      <c r="D43" s="10"/>
+      <c r="E43" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="55"/>
-      <c r="C43" s="14" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B44" s="48"/>
+      <c r="C44" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="11"/>
-      <c r="E43" s="12" t="s">
+      <c r="D44" s="10"/>
+      <c r="E44" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="56"/>
-      <c r="C44" s="15" t="s">
+    <row r="45" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="49"/>
+      <c r="C45" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D44" s="15"/>
-      <c r="E44" s="16" t="s">
+      <c r="D45" s="14"/>
+      <c r="E45" s="15" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="B40:B45"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B18:B23"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B34:B36"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B12:B16"/>
   </mergeCells>

</xml_diff>